<commit_message>
Made a single Roth account in the spreadsheet.
</commit_message>
<xml_diff>
--- a/myStudies/RothProblem.xlsx
+++ b/myStudies/RothProblem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkrat\git\MyStudiesRepo\myStudies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4950CFA6-B21E-4243-8862-BCE1942769FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1F91B2-1AE1-43C1-BA57-B55A67FE290D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="735" activeTab="1" xr2:uid="{61290AE9-9247-4055-A5C3-1005466886B7}"/>
   </bookViews>
@@ -41,6 +41,41 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Thomas Kratzke</author>
+  </authors>
+  <commentList>
+    <comment ref="B54" authorId="0" shapeId="0" xr:uid="{92DBAD28-46AE-46F9-A52C-B4AC725806DE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Thomas Kratzke:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Added Fidelity JWROS, BofA Checking/Savings, and withheld 50K
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Query - https://secure tsp gov/components/CORS/getSharePrices html?G=1" description="Connection to the 'https://secure tsp gov/components/CORS/getSharePrices html?G=1' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
@@ -348,7 +383,7 @@
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,6 +586,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="35">
@@ -2021,11 +2069,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8746EC-93A7-4CC1-BFC6-CA309B41AD35}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8746EC-93A7-4CC1-BFC6-CA309B41AD35}">
   <dimension ref="A1:E269"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2335,7 +2383,7 @@
       </c>
       <c r="B39" s="6">
         <f>0.99*B54</f>
-        <v>111182.23710000001</v>
+        <v>97186.013099999967</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2343,8 +2391,7 @@
         <v>87</v>
       </c>
       <c r="B40" s="6">
-        <f>B53-193342.75</f>
-        <v>-193342.75</v>
+        <v>115839.47999999998</v>
       </c>
       <c r="C40" s="1"/>
     </row>
@@ -2451,8 +2498,8 @@
         <v>88</v>
       </c>
       <c r="B54" s="6">
-        <f>22395.01+124910.28-35000</f>
-        <v>112305.29000000001</v>
+        <f>125772.62+20964.46+1430.61-50000</f>
+        <v>98167.689999999973</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -4571,6 +4618,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId56"/>
+  <legacyDrawing r:id="rId57"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Clean up overwrite/backup mechanism.
</commit_message>
<xml_diff>
--- a/myStudies/RothProblem.xlsx
+++ b/myStudies/RothProblem.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkrat\git\MyStudiesRepo\myStudies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4779E01A-6993-48AF-980A-2840C189DD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA63DB1B-6E23-4E6A-8EF3-0AAA537235CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="735" activeTab="1" xr2:uid="{61290AE9-9247-4055-A5C3-1005466886B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="735" activeTab="2" xr2:uid="{61290AE9-9247-4055-A5C3-1005466886B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Year Parameters" sheetId="39" r:id="rId1"/>
     <sheet name="Owners and Accounts" sheetId="40" r:id="rId2"/>
-    <sheet name="JNT.AC.USA" sheetId="42" r:id="rId3"/>
-    <sheet name="JNT.AC.INT" sheetId="43" r:id="rId4"/>
-    <sheet name="JNT.AC.INV" sheetId="44" r:id="rId5"/>
+    <sheet name="Current Year Tax Info" sheetId="45" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="OI_ROW" localSheetId="0">_xlfn.XMATCH(#REF!,'Current Year Parameters'!#REF!,-1,2)</definedName>
@@ -53,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="104">
   <si>
     <t>Interest Income</t>
   </si>
@@ -331,180 +329,6 @@
     <t>JNT.AC.BoA</t>
   </si>
   <si>
-    <t>TOTALS</t>
-  </si>
-  <si>
-    <t>SPAXX (Core account)</t>
-  </si>
-  <si>
-    <t>Long</t>
-  </si>
-  <si>
-    <t>Holding Period</t>
-  </si>
-  <si>
-    <t>Date Acquired</t>
-  </si>
-  <si>
-    <t>Unrealized % G/L</t>
-  </si>
-  <si>
-    <t>Unrealized G/L</t>
-  </si>
-  <si>
-    <t>Cost Basis/Share</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>ASSOCIATED LOTS</t>
-  </si>
-  <si>
-    <t>10.835 - 24.08</t>
-  </si>
-  <si>
-    <t>20.12 - 20.55</t>
-  </si>
-  <si>
-    <t>OGN</t>
-  </si>
-  <si>
-    <t>309.45 - 461.02</t>
-  </si>
-  <si>
-    <t>457.88 - 461.02</t>
-  </si>
-  <si>
-    <t>9:00 AM ET</t>
-  </si>
-  <si>
-    <t>MSFT</t>
-  </si>
-  <si>
-    <t>99.14 - 134.63</t>
-  </si>
-  <si>
-    <t>125.30 - 127.94</t>
-  </si>
-  <si>
-    <t>8:09 AM ET</t>
-  </si>
-  <si>
-    <t>MRK</t>
-  </si>
-  <si>
-    <t>143.13 - 175.97</t>
-  </si>
-  <si>
-    <t>144.74 - 146.65</t>
-  </si>
-  <si>
-    <t>JNJ</t>
-  </si>
-  <si>
-    <t>64.66 - 84.33</t>
-  </si>
-  <si>
-    <t>80.69 - 81.19</t>
-  </si>
-  <si>
-    <t>IWR</t>
-  </si>
-  <si>
-    <t>102.64 - 132.36</t>
-  </si>
-  <si>
-    <t>128.07 - 129.07</t>
-  </si>
-  <si>
-    <t>IJT</t>
-  </si>
-  <si>
-    <t>87.3201 - 111.57</t>
-  </si>
-  <si>
-    <t>106.17 - 106.97</t>
-  </si>
-  <si>
-    <t>IJR</t>
-  </si>
-  <si>
-    <t>61.15 - 76.20</t>
-  </si>
-  <si>
-    <t>73.4459 - 73.82</t>
-  </si>
-  <si>
-    <t>IEFA</t>
-  </si>
-  <si>
-    <t>Earnings Date</t>
-  </si>
-  <si>
-    <t>% G/L</t>
-  </si>
-  <si>
-    <t>G/L</t>
-  </si>
-  <si>
-    <t>% Tdy G/L</t>
-  </si>
-  <si>
-    <t>Tdy G/L</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Purchase Price</t>
-  </si>
-  <si>
-    <t>52 Wk Range</t>
-  </si>
-  <si>
-    <t>Day Range</t>
-  </si>
-  <si>
-    <t>News</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>Ask</t>
-  </si>
-  <si>
-    <t>Bid</t>
-  </si>
-  <si>
-    <t>% Chg</t>
-  </si>
-  <si>
-    <t>Chg</t>
-  </si>
-  <si>
-    <t>Last</t>
-  </si>
-  <si>
-    <t>% Ext Hrs Chg</t>
-  </si>
-  <si>
-    <t>$ Ext Hrs Chg</t>
-  </si>
-  <si>
-    <t>Ext Hrs Last</t>
-  </si>
-  <si>
-    <t>Symbol</t>
-  </si>
-  <si>
-    <t>07/05/2024 09:26:29 AM ET</t>
-  </si>
-  <si>
-    <t>Positions: Joint WROS - TOD (X82865374)</t>
-  </si>
-  <si>
     <t>Current Value</t>
   </si>
   <si>
@@ -524,6 +348,21 @@
   </si>
   <si>
     <t>Income as % of Income Re-Invested</t>
+  </si>
+  <si>
+    <t>Joint Wros</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Short Term</t>
+  </si>
+  <si>
+    <t>Long Term</t>
+  </si>
+  <si>
+    <t>Tax Adv US SMA</t>
   </si>
 </sst>
 </file>
@@ -537,7 +376,7 @@
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -714,6 +553,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFD41118"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD41118"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="35">
@@ -909,7 +767,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1065,6 +923,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1115,7 +982,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1197,9 +1064,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1214,6 +1081,57 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="8" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="20" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="44" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="21" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="21" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="44" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="21" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="26" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -1282,491 +1200,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5121" name="AutoShape 1" descr="Wash Sale Icon">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEF2DED9-2B27-EB93-E51D-A67BC41D15D2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4267200" y="25003125"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>117</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5122" name="AutoShape 2" descr="52-Week-Indicator is at 99.84%">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4B8765A-E61C-1FC9-69CF-8820218F8BDE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="42557700"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>131</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>132</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5123" name="AutoShape 3" descr="52-Week-Indicator is at 75.26%">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D0B65DA-AD09-BE37-111D-C256C15EAC2C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="45234225"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>143</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>144</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5124" name="AutoShape 4" descr="52-Week-Indicator is at 83.92%">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{653532F2-6E84-AE78-03F9-D6D611EB4496}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="47529750"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>155</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>156</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5125" name="AutoShape 5" descr="52-Week-Indicator is at 78.43%">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19AE38F2-3753-1820-774C-A2B442B161B4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="49825275"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>166</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>167</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5126" name="AutoShape 6" descr="Wash Sale Icon">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56E56296-7ECF-45F2-91B3-3FD4B5A7604E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="51920775"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>167</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>168</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5127" name="AutoShape 7" descr="52-Week-Indicator is at 86.2%">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0AD12DE-09FF-2B05-F714-F57159E72367}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="52120800"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>179</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>180</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5128" name="AutoShape 8" descr="52-Week-Indicator is at 82.21%">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5626C374-8727-D05A-472A-7F40D71C3AD5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="54416325"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>191</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>192</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5129" name="AutoShape 9" descr="52-Week-Indicator is at 7.8%">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F41963CE-A01B-9F3F-7E14-94C41DA97BDF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="56711850"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>203</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>204</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5130" name="AutoShape 10" descr="52-Week-Indicator is at 71.53%">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0EB6689-5C99-FEF8-057A-BA521C8F1C8A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="59007375"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2069,7 +1502,7 @@
   <dimension ref="A1:H235"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:B68"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2089,10 +1522,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="36"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2135,10 +1568,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="38"/>
+      <c r="B7" s="36"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -2173,10 +1606,10 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="40"/>
+      <c r="B12" s="38"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
@@ -2210,7 +1643,7 @@
         <v>383900</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>0.32</v>
       </c>
@@ -2218,7 +1651,7 @@
         <v>487450</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>0.35</v>
       </c>
@@ -2226,68 +1659,72 @@
         <v>731200</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>0.37</v>
       </c>
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="str">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="str">
         <f>_xlfn.CONCAT(A12," 2026")</f>
         <v>Ordinary Rates 2026</v>
       </c>
-      <c r="B20" s="40"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="38"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>0.1</v>
       </c>
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>0.15</v>
       </c>
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>0.25</v>
       </c>
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>0.28000000000000003</v>
       </c>
       <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="1">
+        <f>(A40-1)*(2*12*B9)</f>
+        <v>6708.48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>0.33</v>
       </c>
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>0.35</v>
       </c>
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>0.39600000000000002</v>
       </c>
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="40"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="38"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>0</v>
       </c>
@@ -2295,7 +1732,7 @@
         <v>94050</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>0.15</v>
       </c>
@@ -2303,17 +1740,17 @@
         <v>583750</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>0.2</v>
       </c>
       <c r="B31" s="5"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="40"/>
+      <c r="B32" s="38"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
@@ -2338,10 +1775,10 @@
       <c r="B35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="40"/>
+      <c r="B36" s="38"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
@@ -2391,10 +1828,10 @@
       <c r="B42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="40"/>
+      <c r="B43" s="38"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="14">
@@ -2591,10 +2028,10 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="41" t="s">
+      <c r="A68" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B68" s="42"/>
+      <c r="B68" s="40"/>
     </row>
     <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2638,8 +2075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E76ACA-50AD-44D7-AB75-CC74A26DA038}">
   <dimension ref="A1:D180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,10 +2094,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="36"/>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2697,10 +2134,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="36"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -2725,10 +2162,10 @@
       <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="38"/>
+      <c r="B10" s="36"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -2764,10 +2201,10 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="38"/>
+      <c r="B15" s="36"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -2795,10 +2232,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="38"/>
+      <c r="B19" s="36"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -2825,10 +2262,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="38"/>
+      <c r="B23" s="36"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -2847,10 +2284,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="38"/>
+      <c r="B26" s="36"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -2863,15 +2300,15 @@
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="38"/>
+      <c r="B28" s="36"/>
       <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>150</v>
+        <v>92</v>
       </c>
       <c r="B29" s="5">
         <v>40610.959999999999</v>
@@ -2903,7 +2340,10 @@
       <c r="B32" s="2">
         <v>17.2</v>
       </c>
-      <c r="C32" s="3"/>
+      <c r="C32" s="35">
+        <f>B31/B32+290000+B16+B11+B27+75000</f>
+        <v>485051.92906976747</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -2915,15 +2355,15 @@
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="38"/>
+      <c r="B34" s="36"/>
       <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>150</v>
+        <v>92</v>
       </c>
       <c r="B35" s="5">
         <v>1970046.2100000002</v>
@@ -2946,15 +2386,15 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="38"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>150</v>
+        <v>92</v>
       </c>
       <c r="B39" s="5">
         <v>1009000</v>
@@ -2978,14 +2418,14 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="B42" s="38"/>
+      <c r="B42" s="36"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>150</v>
+        <v>92</v>
       </c>
       <c r="B43" s="5">
         <v>310024.56999999995</v>
@@ -2993,7 +2433,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>151</v>
+        <v>93</v>
       </c>
       <c r="B44" s="5">
         <v>100000</v>
@@ -3001,7 +2441,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>152</v>
+        <v>94</v>
       </c>
       <c r="B45" s="7">
         <v>0.05</v>
@@ -3010,7 +2450,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>153</v>
+        <v>95</v>
       </c>
       <c r="B46" s="7">
         <v>0.08</v>
@@ -3019,7 +2459,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="B47" s="7">
         <v>0.03</v>
@@ -3028,7 +2468,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>155</v>
+        <v>97</v>
       </c>
       <c r="B48" s="7">
         <v>0.02</v>
@@ -3037,7 +2477,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>156</v>
+        <v>98</v>
       </c>
       <c r="B49" s="7">
         <v>0.04</v>
@@ -3045,14 +2485,14 @@
       <c r="C49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="38" t="s">
+      <c r="A50" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="38"/>
+      <c r="B50" s="36"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>150</v>
+        <v>92</v>
       </c>
       <c r="B51" s="6">
         <v>649728.07000000007</v>
@@ -3067,20 +2507,20 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="41" t="s">
+      <c r="A53" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B53" s="42"/>
+      <c r="B53" s="40"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="7"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="38" t="s">
+      <c r="A55" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="B55" s="38"/>
+      <c r="B55" s="36"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
@@ -3771,1107 +3211,799 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A05454-6C22-4808-8894-C2A89CDBBDC7}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2975635C-74C3-4ED3-85A2-DDB645904B01}">
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D618011E-9A97-457D-AEBE-A2A00015444E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455D7C0F-CD6C-4DB6-AE0A-F642FCFFAEED}">
-  <dimension ref="A1:U39"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>4541.92</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2">
+        <v>4541.92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" t="s">
-        <v>145</v>
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>4541.92</v>
       </c>
       <c r="D4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H4" t="s">
-        <v>140</v>
-      </c>
-      <c r="I4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K4" t="s">
-        <v>137</v>
-      </c>
-      <c r="L4" t="s">
-        <v>136</v>
-      </c>
-      <c r="M4" t="s">
-        <v>135</v>
-      </c>
-      <c r="N4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4">
+        <v>4541.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>75436.960000000006</v>
+      </c>
+      <c r="D13">
+        <v>75436.960000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>75436.960000000006</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>75436.960000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25">
+        <v>4541.92</v>
+      </c>
+      <c r="D25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25">
+        <v>4541.92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <v>2902.52</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26">
+        <v>2902.52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <v>1639.4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27">
+        <v>1639.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="D38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="D44" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="O4" t="s">
-        <v>134</v>
-      </c>
-      <c r="P4" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>132</v>
-      </c>
-      <c r="R4" t="s">
-        <v>131</v>
-      </c>
-      <c r="S4" t="s">
-        <v>130</v>
-      </c>
-      <c r="T4" t="s">
-        <v>129</v>
-      </c>
-      <c r="U4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5">
-        <v>74.42</v>
-      </c>
-      <c r="C5">
-        <v>0.64</v>
-      </c>
-      <c r="D5">
-        <v>0.87</v>
-      </c>
-      <c r="E5">
-        <v>73.78</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>74.319999999999993</v>
-      </c>
-      <c r="I5">
-        <v>74.42</v>
-      </c>
-      <c r="J5" s="37">
-        <v>54422</v>
-      </c>
-      <c r="L5" t="s">
-        <v>126</v>
-      </c>
-      <c r="M5" t="s">
-        <v>125</v>
-      </c>
-      <c r="N5">
-        <v>483</v>
-      </c>
-      <c r="O5">
-        <v>60.57</v>
-      </c>
-      <c r="P5">
-        <v>35635.74</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="B45" s="1">
+        <v>4541.92</v>
+      </c>
+      <c r="D45" t="s">
+        <v>100</v>
+      </c>
+      <c r="E45">
+        <v>4541.92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>101</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" s="1">
+        <v>75436.960000000006</v>
+      </c>
+      <c r="D47" t="s">
+        <v>102</v>
+      </c>
+      <c r="E47">
+        <v>75436.960000000006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="53"/>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="42">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="44"/>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="46">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A61" s="54" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A62" s="55">
+        <v>-1148.6199999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="56">
+        <v>-1149.78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64" s="49">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A65" s="54" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="R5" t="s">
+    </row>
+    <row r="67" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="S5" s="35">
-        <v>6382.83</v>
-      </c>
-      <c r="T5">
-        <v>21.82</v>
-      </c>
-      <c r="U5" t="s">
+    </row>
+    <row r="68" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" s="50" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>483</v>
-      </c>
-      <c r="B8">
-        <v>60.57</v>
-      </c>
-      <c r="C8" s="35">
-        <v>6382.83</v>
-      </c>
-      <c r="D8">
-        <v>21.82</v>
-      </c>
-      <c r="E8" s="36">
-        <v>43609</v>
-      </c>
-      <c r="F8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B9">
-        <v>106.04</v>
-      </c>
-      <c r="C9">
-        <v>-0.3</v>
-      </c>
-      <c r="D9">
-        <v>-0.28000000000000003</v>
-      </c>
-      <c r="E9">
-        <v>106.34</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>105.83</v>
-      </c>
-      <c r="I9">
-        <v>106.77</v>
-      </c>
-      <c r="J9">
-        <v>874</v>
-      </c>
-      <c r="L9" t="s">
-        <v>123</v>
-      </c>
-      <c r="M9" t="s">
-        <v>122</v>
-      </c>
-      <c r="N9">
-        <v>281</v>
-      </c>
-      <c r="O9">
-        <v>81.290000000000006</v>
-      </c>
-      <c r="P9">
-        <v>29881.54</v>
-      </c>
-      <c r="Q9" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B69" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="R9" t="s">
-        <v>44</v>
-      </c>
-      <c r="S9" s="35">
-        <v>7039.05</v>
-      </c>
-      <c r="T9">
-        <v>30.82</v>
-      </c>
-      <c r="U9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11" t="s">
-        <v>96</v>
-      </c>
-      <c r="F11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>281</v>
-      </c>
-      <c r="B12">
-        <v>81.290000000000006</v>
-      </c>
-      <c r="C12" s="35">
-        <v>7039.05</v>
-      </c>
-      <c r="D12">
-        <v>30.82</v>
-      </c>
-      <c r="E12" s="36">
-        <v>43803</v>
-      </c>
-      <c r="F12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13">
-        <v>121.85</v>
-      </c>
-      <c r="C13">
-        <v>-6.41</v>
-      </c>
-      <c r="D13">
-        <v>-5</v>
-      </c>
-      <c r="E13">
-        <v>128.26</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>120.93</v>
-      </c>
-      <c r="I13">
-        <v>135.54</v>
-      </c>
-      <c r="J13">
-        <v>139</v>
-      </c>
-      <c r="L13" t="s">
-        <v>120</v>
-      </c>
-      <c r="M13" t="s">
-        <v>119</v>
-      </c>
-      <c r="N13">
-        <v>180</v>
-      </c>
-      <c r="O13">
-        <v>90.19</v>
-      </c>
-      <c r="P13">
-        <v>23086.799999999999</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>44</v>
-      </c>
-      <c r="R13" t="s">
-        <v>44</v>
-      </c>
-      <c r="S13" s="35">
-        <v>6852.55</v>
-      </c>
-      <c r="T13">
-        <v>42.21</v>
-      </c>
-      <c r="U13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>140</v>
-      </c>
-      <c r="B16">
-        <v>86.22</v>
-      </c>
-      <c r="C16" s="35">
-        <v>5885.6</v>
-      </c>
-      <c r="D16">
-        <v>48.76</v>
-      </c>
-      <c r="E16" s="36">
-        <v>43999</v>
-      </c>
-      <c r="F16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>40</v>
-      </c>
-      <c r="B17">
-        <v>104.09</v>
-      </c>
-      <c r="C17">
-        <v>966.95</v>
-      </c>
-      <c r="D17">
-        <v>23.22</v>
-      </c>
-      <c r="E17" s="36">
-        <v>43795</v>
-      </c>
-      <c r="F17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>118</v>
-      </c>
-      <c r="B18">
-        <v>80.83</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>80.83</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>80.709999999999994</v>
-      </c>
-      <c r="I18">
-        <v>81.11</v>
-      </c>
-      <c r="J18">
-        <v>30</v>
-      </c>
-      <c r="L18" t="s">
-        <v>117</v>
-      </c>
-      <c r="M18" t="s">
-        <v>116</v>
-      </c>
-      <c r="N18">
-        <v>280</v>
-      </c>
-      <c r="O18">
-        <v>53.83</v>
-      </c>
-      <c r="P18">
-        <v>22632.400000000001</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>44</v>
-      </c>
-      <c r="R18" t="s">
-        <v>44</v>
-      </c>
-      <c r="S18" s="35">
-        <v>7560</v>
-      </c>
-      <c r="T18">
-        <v>50.16</v>
-      </c>
-      <c r="U18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E20" t="s">
-        <v>96</v>
-      </c>
-      <c r="F20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>280</v>
-      </c>
-      <c r="B21">
-        <v>53.83</v>
-      </c>
-      <c r="C21" s="35">
-        <v>7560</v>
-      </c>
-      <c r="D21">
-        <v>50.16</v>
-      </c>
-      <c r="E21" s="36">
-        <v>43609</v>
-      </c>
-      <c r="F21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>115</v>
-      </c>
-      <c r="B22">
-        <v>145.80000000000001</v>
-      </c>
-      <c r="C22">
-        <v>0.11</v>
-      </c>
-      <c r="D22">
-        <v>0.08</v>
-      </c>
-      <c r="E22">
-        <v>145.69</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>145.62</v>
-      </c>
-      <c r="I22">
-        <v>145.83000000000001</v>
-      </c>
-      <c r="J22" s="37">
-        <v>8659</v>
-      </c>
-      <c r="L22" t="s">
-        <v>114</v>
-      </c>
-      <c r="M22" t="s">
-        <v>113</v>
-      </c>
-      <c r="N22">
-        <v>100</v>
-      </c>
-      <c r="O22">
-        <v>49.97</v>
-      </c>
-      <c r="P22">
-        <v>14569</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>44</v>
-      </c>
-      <c r="R22" t="s">
-        <v>44</v>
-      </c>
-      <c r="S22" s="35">
-        <v>9572.01</v>
-      </c>
-      <c r="T22">
-        <v>191.56</v>
-      </c>
-      <c r="U22" s="36">
-        <v>45490</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>100</v>
-      </c>
-      <c r="B24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" t="s">
-        <v>96</v>
-      </c>
-      <c r="F24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>100</v>
-      </c>
-      <c r="B25">
-        <v>49.97</v>
-      </c>
-      <c r="C25" s="35">
-        <v>9572.01</v>
-      </c>
-      <c r="D25">
-        <v>191.56</v>
-      </c>
-      <c r="E25" s="36">
-        <v>37855</v>
-      </c>
-      <c r="F25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>112</v>
-      </c>
-      <c r="B26">
-        <v>126.005</v>
-      </c>
-      <c r="C26">
-        <v>0.155</v>
-      </c>
-      <c r="D26">
-        <v>0.12</v>
-      </c>
-      <c r="E26">
-        <v>125.85</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>125.5</v>
-      </c>
-      <c r="I26">
-        <v>126.5</v>
-      </c>
-      <c r="J26" s="37">
-        <v>2369</v>
-      </c>
-      <c r="K26" t="s">
-        <v>111</v>
-      </c>
-      <c r="L26" t="s">
-        <v>110</v>
-      </c>
-      <c r="M26" t="s">
-        <v>109</v>
-      </c>
-      <c r="N26">
-        <v>400</v>
-      </c>
-      <c r="O26">
-        <v>48.31</v>
-      </c>
-      <c r="P26">
-        <v>50340</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>44</v>
-      </c>
-      <c r="R26" t="s">
-        <v>44</v>
-      </c>
-      <c r="S26" s="35">
-        <v>31015.45</v>
-      </c>
-      <c r="T26">
-        <v>160.5</v>
-      </c>
-      <c r="U26" s="36">
-        <v>45503</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" t="s">
-        <v>99</v>
-      </c>
-      <c r="C28" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" t="s">
-        <v>97</v>
-      </c>
-      <c r="E28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>400</v>
-      </c>
-      <c r="B29">
-        <v>48.31</v>
-      </c>
-      <c r="C29" s="35">
-        <v>31015.45</v>
-      </c>
-      <c r="D29">
-        <v>160.5</v>
-      </c>
-      <c r="E29" s="36">
-        <v>42290</v>
-      </c>
-      <c r="F29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>108</v>
-      </c>
-      <c r="B30">
-        <v>460.21</v>
-      </c>
-      <c r="C30">
-        <v>-0.56000000000000005</v>
-      </c>
-      <c r="D30">
-        <v>-0.12</v>
-      </c>
-      <c r="E30">
-        <v>460.77</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>460.2</v>
-      </c>
-      <c r="I30">
-        <v>460.26</v>
-      </c>
-      <c r="J30" s="37">
-        <v>378498</v>
-      </c>
-      <c r="K30" t="s">
-        <v>107</v>
-      </c>
-      <c r="L30" t="s">
-        <v>106</v>
-      </c>
-      <c r="M30" t="s">
-        <v>105</v>
-      </c>
-      <c r="N30">
-        <v>300</v>
-      </c>
-      <c r="O30">
-        <v>23.83</v>
-      </c>
-      <c r="P30">
-        <v>138231</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>44</v>
-      </c>
-      <c r="R30" t="s">
-        <v>44</v>
-      </c>
-      <c r="S30" s="35">
-        <v>131082.51</v>
-      </c>
-      <c r="T30" s="35">
-        <v>1833.71</v>
-      </c>
-      <c r="U30" s="36">
-        <v>45496</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" t="s">
-        <v>96</v>
-      </c>
-      <c r="F32" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>300</v>
-      </c>
-      <c r="B33">
-        <v>23.83</v>
-      </c>
-      <c r="C33" s="35">
-        <v>131082.51</v>
-      </c>
-      <c r="D33" s="35">
-        <v>1833.71</v>
-      </c>
-      <c r="E33" s="36">
-        <v>37658</v>
-      </c>
-      <c r="F33" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>104</v>
-      </c>
-      <c r="B34">
-        <v>20.32</v>
-      </c>
-      <c r="C34">
-        <v>0.01</v>
-      </c>
-      <c r="D34">
-        <v>0.05</v>
-      </c>
-      <c r="E34">
-        <v>20.309999999999999</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>20.309999999999999</v>
-      </c>
-      <c r="I34">
-        <v>21.01</v>
-      </c>
-      <c r="J34">
-        <v>4</v>
-      </c>
-      <c r="L34" t="s">
-        <v>103</v>
-      </c>
-      <c r="M34" t="s">
-        <v>102</v>
-      </c>
-      <c r="N34">
-        <v>40</v>
-      </c>
-      <c r="O34">
-        <v>24.19</v>
-      </c>
-      <c r="P34">
-        <v>812.4</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>44</v>
-      </c>
-      <c r="R34" t="s">
-        <v>44</v>
-      </c>
-      <c r="S34">
-        <v>-155</v>
-      </c>
-      <c r="T34">
-        <v>-16.02</v>
-      </c>
-      <c r="U34" s="36">
-        <v>45510</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>100</v>
-      </c>
-      <c r="B36" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" t="s">
-        <v>97</v>
-      </c>
-      <c r="E36" t="s">
-        <v>96</v>
-      </c>
-      <c r="F36" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>40</v>
-      </c>
-      <c r="B37">
-        <v>24.18</v>
-      </c>
-      <c r="C37">
-        <v>-155</v>
-      </c>
-      <c r="D37">
-        <v>-16.02</v>
-      </c>
-      <c r="E37" s="36">
-        <v>42290</v>
-      </c>
-      <c r="F37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" t="s">
-        <v>44</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38" t="s">
-        <v>44</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38" t="s">
-        <v>44</v>
-      </c>
-      <c r="L38" t="s">
-        <v>44</v>
-      </c>
-      <c r="N38" s="35">
-        <v>126318.94</v>
-      </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-      <c r="P38">
-        <v>126318.94</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>44</v>
-      </c>
-      <c r="R38" t="s">
-        <v>44</v>
-      </c>
-      <c r="S38" t="s">
-        <v>44</v>
-      </c>
-      <c r="T38" t="s">
-        <v>44</v>
-      </c>
-      <c r="U38" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>92</v>
-      </c>
-      <c r="N39">
-        <v>0</v>
-      </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-      <c r="P39">
-        <v>441507.82</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>44</v>
-      </c>
-      <c r="R39" t="s">
-        <v>44</v>
-      </c>
-      <c r="S39" s="35">
-        <v>199349.4</v>
-      </c>
-      <c r="T39">
-        <v>172.09</v>
+    </row>
+    <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A70" s="54" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" s="49">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A50:B50"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A52" r:id="rId1" display="javascript:void(0)" xr:uid="{4675DE9B-AE5B-4652-8FE9-9BCE10FBE401}"/>
+    <hyperlink ref="A55" r:id="rId2" display="javascript:void(0)" xr:uid="{5723C74E-E4A2-410D-87F0-99A3A2F509BA}"/>
+    <hyperlink ref="A56" r:id="rId3" display="javascript:void(0)" xr:uid="{4257DF38-4119-4B5F-B23A-7707AF920A52}"/>
+    <hyperlink ref="A57" r:id="rId4" display="javascript:void(0)" xr:uid="{FFA45F7C-DA21-4B94-AAD9-B78AB81EED94}"/>
+    <hyperlink ref="A59" r:id="rId5" display="javascript:void(0)" xr:uid="{01F1C6DD-6413-430F-B2EE-198DFB91063B}"/>
+    <hyperlink ref="A60" r:id="rId6" display="javascript:void(0)" xr:uid="{288081C4-A4DF-4DAD-9243-97675A9ECBFB}"/>
+    <hyperlink ref="A63" r:id="rId7" display="javascript:void(0)" xr:uid="{FD921898-6DF8-40E3-9207-EB8B4E549D7A}"/>
+    <hyperlink ref="A64" r:id="rId8" display="javascript:void(0)" xr:uid="{A562AEF9-4D32-47FC-8D0E-370FD0470214}"/>
+    <hyperlink ref="A66" r:id="rId9" display="javascript:void(0)" xr:uid="{F7B383B2-6884-4AEE-9515-BD8555012B25}"/>
+    <hyperlink ref="A67" r:id="rId10" display="javascript:void(0)" xr:uid="{59E15290-449D-4801-A815-C542F7FD034B}"/>
+    <hyperlink ref="A68" r:id="rId11" display="javascript:void(0)" xr:uid="{8B7CA53B-C7F1-4A4A-AFB1-3668B4C2F505}"/>
+    <hyperlink ref="A69" r:id="rId12" display="javascript:void(0)" xr:uid="{7D8BE727-F452-4283-B084-5CCAE1051C29}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>